<commit_message>
The issue with rollers in step details...
is caused by the style dropDownListStyle, need to understand how to solve this
</commit_message>
<xml_diff>
--- a/resources/FontUsage.xlsx
+++ b/resources/FontUsage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescoprochilo/Documents/Arduino/FilMachine_Again/TheBeginningObject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescoprochilo/Documents/Arduino/FilMachine_Again/TheBeginningObject/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886C9AA0-BCD0-154E-BBE3-C8989B502FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E91114-2F35-B84C-AE69-CFE11CAC400F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>